<commit_message>
Fix new progbook generation on FE
</commit_message>
<xml_diff>
--- a/atomica/library/tb_progbook.xlsx
+++ b/atomica/library/tb_progbook.xlsx
@@ -37383,1266 +37383,636 @@
       <formula>'Program targeting'!$G$14&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="420">
+  <dataValidations count="210">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D26">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D27">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D30">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D31">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D32">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D33">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C34">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D34">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C37">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D37">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C38">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D38">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D39">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C40">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D40">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C41">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D41">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C44">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D44">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C45">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D45">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C46">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D46">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D47">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C48">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D48">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D51">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C52">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D52">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C53">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D53">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C54">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D54">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C55">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D55">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C58">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D58">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C59">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D59">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C60">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D60">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C61">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D61">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C62">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D62">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C65">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D65">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C66">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D66">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C67">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D67">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C68">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D68">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C69">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D69">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C72">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D72">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C73">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D73">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C74">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D74">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C75">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D75">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C76">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D76">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C79">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D79">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C80">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D80">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C81">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D81">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C82">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D82">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C83">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D83">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C86">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D86">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C87">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D87">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C88">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D88">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C89">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D89">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C90">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D90">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C93">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D93">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C94">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D94">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C95">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D95">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C96">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D96">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C97">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D97">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C100">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D100">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C101">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D101">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C102">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D102">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C103">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D103">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C104">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D104">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C107">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D107">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C108">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D108">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C109">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D109">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C110">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D110">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C111">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D111">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C114">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D114">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C115">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D115">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C116">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D116">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C117">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D117">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C118">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D118">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C121">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D121">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C122">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D122">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C123">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D123">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C124">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D124">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C125">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D125">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C128">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D128">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C129">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D129">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C130">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D130">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C131">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D131">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C132">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D132">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C135">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D135">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C136">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D136">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C137">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D137">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C138">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D138">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C139">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D139">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C142">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D142">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C143">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D143">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C144">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D144">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C145">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D145">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C146">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D146">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C149">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D149">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C150">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D150">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C151">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D151">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C152">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D152">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C153">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D153">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C156">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D156">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C157">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D157">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C158">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D158">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C159">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D159">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C160">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D160">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C163">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D163">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C164">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D164">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C165">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D165">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C166">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D166">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C167">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D167">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C170">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D170">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C171">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D171">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C172">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D172">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C173">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D173">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C174">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D174">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C177">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D177">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C178">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D178">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C179">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D179">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C180">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D180">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C181">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D181">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C184">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D184">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C185">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D185">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C186">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D186">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C187">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D187">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C188">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D188">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C191">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D191">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C192">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D192">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C193">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D193">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C194">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D194">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C195">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D195">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C198">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D198">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C199">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D199">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C200">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D200">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C201">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D201">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C202">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D202">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C205">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D205">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C206">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D206">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C207">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D207">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C208">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D208">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C209">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D209">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C212">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D212">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C213">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D213">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C214">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D214">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C215">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D215">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C216">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D216">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C219">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D219">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C220">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D220">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C221">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D221">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C222">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D222">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C223">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D223">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C226">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D226">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C227">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D227">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C228">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D228">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C229">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D229">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C230">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D230">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C233">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D233">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C234">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D234">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C235">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D235">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C236">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D236">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C237">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D237">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C240">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D240">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C241">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D241">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C242">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D242">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C243">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D243">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C244">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D244">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C247">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D247">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C248">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D248">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C249">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D249">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C250">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D250">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C251">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D251">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C254">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D254">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C255">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D255">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C256">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D256">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C257">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D257">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C258">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D258">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C261">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D261">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C262">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D262">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C263">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D263">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C264">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D264">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C265">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D265">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C268">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D268">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C269">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D269">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C270">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D270">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C271">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D271">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C272">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D272">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C275">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D275">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C276">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D276">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C277">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D277">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C278">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D278">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C279">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D279">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C282">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D282">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C283">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D283">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C284">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D284">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C285">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D285">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C286">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D286">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C289">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D289">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C290">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D290">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C291">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D291">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C292">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D292">
-      <formula1>"Synergistic,Best"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C293">
       <formula1>"Random,Additive,Nested"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D293">
-      <formula1>"Synergistic,Best"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>